<commit_message>
Ziterfassig grad na gmacht
</commit_message>
<xml_diff>
--- a/Zeiterfassung/19FS_pro2E_Team_x_Personalkosten_Tracking.xlsx
+++ b/Zeiterfassung/19FS_pro2E_Team_x_Personalkosten_Tracking.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B0993538-78A6-4517-9735-E849F1DDC408}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3642EEA9-1CDE-EE4E-9BF1-4079391156C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kosten" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,15 @@
     <sheet name="Status-3" sheetId="5" r:id="rId4"/>
     <sheet name="Status-4" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2110,13 +2118,13 @@
                   <c:v>1.292</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4337,28 +4345,28 @@
                   <c:v>1.292</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6657,46 +6665,46 @@
                   <c:v>1.292</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9079,58 +9087,58 @@
                   <c:v>1.292</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.5360000000000005</c:v>
+                  <c:v>4.3520000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10320,33 +10328,33 @@
   <dimension ref="B2:AA112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="10" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="10" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
+      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="8.6640625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="3.44140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="3.5" style="1" customWidth="1"/>
     <col min="27" max="27" width="8.6640625" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.109375" style="1"/>
+    <col min="28" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2"/>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
@@ -10354,7 +10362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
@@ -10362,7 +10370,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C7" s="1" t="s">
         <v>65</v>
       </c>
@@ -10371,10 +10379,10 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.15">
       <c r="AA8" s="16"/>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.15">
       <c r="J9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -10385,7 +10393,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="E10" s="13" t="s">
         <v>3</v>
       </c>
@@ -10454,7 +10462,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
@@ -10485,7 +10493,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -10503,13 +10511,13 @@
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B14" s="24" t="s">
         <v>0</v>
       </c>
@@ -10585,7 +10593,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C15" s="8" t="s">
         <v>2</v>
       </c>
@@ -10676,7 +10684,7 @@
       </c>
       <c r="AA15" s="5"/>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C16" s="9" t="s">
         <v>38</v>
       </c>
@@ -10772,7 +10780,7 @@
         <v>12.375999999999996</v>
       </c>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B17" s="15" t="s">
         <v>47</v>
       </c>
@@ -10867,10 +10875,10 @@
         <v>12.375999999999996</v>
       </c>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.15">
       <c r="AA18" s="22"/>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B19" s="24" t="s">
         <v>41</v>
       </c>
@@ -10930,7 +10938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C20" s="12" t="s">
         <v>43</v>
       </c>
@@ -10965,7 +10973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C21" s="12" t="s">
         <v>44</v>
       </c>
@@ -10998,7 +11006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C22" s="8" t="s">
         <v>37</v>
       </c>
@@ -11087,7 +11095,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C23" s="8" t="s">
         <v>2</v>
       </c>
@@ -11178,7 +11186,7 @@
       </c>
       <c r="AA23" s="5"/>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C24" s="9" t="s">
         <v>38</v>
       </c>
@@ -11274,7 +11282,7 @@
         <v>6.6639999999999979</v>
       </c>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B25" s="15" t="s">
         <v>48</v>
       </c>
@@ -11369,13 +11377,13 @@
         <v>6.6639999999999979</v>
       </c>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C27" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B28" s="24" t="s">
         <v>0</v>
       </c>
@@ -11425,7 +11433,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C29" s="8" t="s">
         <v>2</v>
       </c>
@@ -11516,7 +11524,7 @@
       </c>
       <c r="AA29" s="5"/>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C30" s="9" t="s">
         <v>38</v>
       </c>
@@ -11612,7 +11620,7 @@
         <v>11.016</v>
       </c>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B31" s="15" t="s">
         <v>51</v>
       </c>
@@ -11707,7 +11715,7 @@
         <v>11.016</v>
       </c>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B33" s="24" t="s">
         <v>41</v>
       </c>
@@ -11751,7 +11759,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B34" s="6"/>
       <c r="C34" s="12" t="s">
         <v>68</v>
@@ -11786,7 +11794,7 @@
       <c r="Y34" s="20"/>
       <c r="AA34" s="23"/>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B35" s="6"/>
       <c r="C35" s="12" t="s">
         <v>69</v>
@@ -11801,7 +11809,9 @@
       <c r="G35" s="20">
         <v>1</v>
       </c>
-      <c r="H35" s="20"/>
+      <c r="H35" s="20">
+        <v>12</v>
+      </c>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
       <c r="K35" s="20"/>
@@ -11821,7 +11831,7 @@
       <c r="Y35" s="20"/>
       <c r="AA35" s="23"/>
     </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B36" s="6"/>
       <c r="C36" s="12" t="s">
         <v>71</v>
@@ -11854,7 +11864,7 @@
       <c r="Y36" s="20"/>
       <c r="AA36" s="23"/>
     </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C37" s="12" t="s">
         <v>46</v>
       </c>
@@ -11887,7 +11897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C38" s="12" t="s">
         <v>49</v>
       </c>
@@ -11920,7 +11930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C39" s="8" t="s">
         <v>37</v>
       </c>
@@ -11939,7 +11949,7 @@
       </c>
       <c r="H39" s="21">
         <f t="shared" ref="H39" si="79">SUM(H33:H38)</f>
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="I39" s="21">
         <f t="shared" ref="I39" si="80">SUM(I33:I38)</f>
@@ -12011,10 +12021,10 @@
       </c>
       <c r="AA39" s="21">
         <f t="shared" si="76"/>
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C40" s="8" t="s">
         <v>2</v>
       </c>
@@ -12033,79 +12043,79 @@
       </c>
       <c r="H40" s="19">
         <f t="shared" ref="H40" si="98">G40+H39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="I40" s="19">
         <f t="shared" ref="I40" si="99">H40+I39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J40" s="19">
         <f t="shared" ref="J40" si="100">I40+J39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="K40" s="19">
         <f t="shared" ref="K40" si="101">J40+K39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="L40" s="19">
         <f t="shared" ref="L40" si="102">K40+L39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="M40" s="19">
         <f t="shared" ref="M40" si="103">L40+M39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="N40" s="19">
         <f t="shared" ref="N40" si="104">M40+N39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="O40" s="19">
         <f t="shared" ref="O40" si="105">N40+O39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="P40" s="19">
         <f t="shared" ref="P40" si="106">O40+P39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="Q40" s="19">
         <f t="shared" ref="Q40" si="107">P40+Q39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="R40" s="19">
         <f t="shared" ref="R40" si="108">Q40+R39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="S40" s="19">
         <f t="shared" ref="S40" si="109">R40+S39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="T40" s="19">
         <f t="shared" ref="T40" si="110">S40+T39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="U40" s="19">
         <f t="shared" ref="U40" si="111">T40+U39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="V40" s="19">
         <f t="shared" ref="V40" si="112">U40+V39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="W40" s="19">
         <f t="shared" ref="W40" si="113">V40+W39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="X40" s="19">
         <f t="shared" ref="X40" si="114">W40+X39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="Y40" s="19">
         <f t="shared" ref="Y40" si="115">X40+Y39</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="AA40" s="5"/>
     </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C41" s="9" t="s">
         <v>38</v>
       </c>
@@ -12126,7 +12136,7 @@
       </c>
       <c r="H41" s="11">
         <f t="shared" si="116"/>
-        <v>2.2440000000000002</v>
+        <v>3.06</v>
       </c>
       <c r="I41" s="11">
         <f t="shared" si="116"/>
@@ -12198,10 +12208,10 @@
       </c>
       <c r="AA41" s="11">
         <f>SUM(E41:Y41)</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
     </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B42" s="15" t="s">
         <v>52</v>
       </c>
@@ -12225,84 +12235,84 @@
       </c>
       <c r="H42" s="11">
         <f t="shared" ref="H42" si="118">G42+H41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="I42" s="11">
         <f t="shared" ref="I42" si="119">H42+I41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="J42" s="11">
         <f t="shared" ref="J42" si="120">I42+J41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="K42" s="11">
         <f t="shared" ref="K42" si="121">J42+K41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="L42" s="11">
         <f t="shared" ref="L42" si="122">K42+L41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="M42" s="11">
         <f t="shared" ref="M42" si="123">L42+M41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="N42" s="11">
         <f t="shared" ref="N42" si="124">M42+N41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="O42" s="11">
         <f t="shared" ref="O42" si="125">N42+O41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="P42" s="11">
         <f t="shared" ref="P42" si="126">O42+P41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="Q42" s="11">
         <f t="shared" ref="Q42" si="127">P42+Q41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="R42" s="11">
         <f t="shared" ref="R42" si="128">Q42+R41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="S42" s="11">
         <f t="shared" ref="S42" si="129">R42+S41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="T42" s="11">
         <f t="shared" ref="T42" si="130">S42+T41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="U42" s="11">
         <f t="shared" ref="U42" si="131">T42+U41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="V42" s="11">
         <f t="shared" ref="V42" si="132">U42+V41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="W42" s="11">
         <f t="shared" ref="W42" si="133">V42+W41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="X42" s="11">
         <f t="shared" ref="X42" si="134">W42+X41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
       <c r="Y42" s="11">
         <f t="shared" ref="Y42" si="135">X42+Y41</f>
-        <v>3.5360000000000005</v>
+        <v>4.3520000000000003</v>
       </c>
     </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C44" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B45" s="24" t="s">
         <v>0</v>
       </c>
@@ -12354,7 +12364,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C46" s="8" t="s">
         <v>2</v>
       </c>
@@ -12445,7 +12455,7 @@
       </c>
       <c r="AA46" s="5"/>
     </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C47" s="9" t="s">
         <v>38</v>
       </c>
@@ -12541,7 +12551,7 @@
         <v>10.879999999999999</v>
       </c>
     </row>
-    <row r="48" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B48" s="15" t="s">
         <v>57</v>
       </c>
@@ -12636,7 +12646,7 @@
         <v>10.879999999999999</v>
       </c>
     </row>
-    <row r="50" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B50" s="24" t="s">
         <v>41</v>
       </c>
@@ -12672,7 +12682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B51" s="6"/>
       <c r="C51" s="12" t="s">
         <v>43</v>
@@ -12709,7 +12719,7 @@
       <c r="Y51" s="20"/>
       <c r="AA51" s="23"/>
     </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B52" s="6"/>
       <c r="C52" s="12" t="s">
         <v>44</v>
@@ -12746,7 +12756,7 @@
       <c r="Y52" s="20"/>
       <c r="AA52" s="23"/>
     </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B53" s="6"/>
       <c r="C53" s="12" t="s">
         <v>45</v>
@@ -12783,7 +12793,7 @@
       <c r="Y53" s="20"/>
       <c r="AA53" s="23"/>
     </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C54" s="12" t="s">
         <v>46</v>
       </c>
@@ -12816,7 +12826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C55" s="12" t="s">
         <v>49</v>
       </c>
@@ -12849,7 +12859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C56" s="8" t="s">
         <v>37</v>
       </c>
@@ -12943,7 +12953,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C57" s="8" t="s">
         <v>2</v>
       </c>
@@ -13034,7 +13044,7 @@
       </c>
       <c r="AA57" s="5"/>
     </row>
-    <row r="58" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C58" s="9" t="s">
         <v>38</v>
       </c>
@@ -13130,7 +13140,7 @@
         <v>4.3520000000000003</v>
       </c>
     </row>
-    <row r="59" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B59" s="15" t="s">
         <v>58</v>
       </c>
@@ -13225,13 +13235,13 @@
         <v>4.3520000000000003</v>
       </c>
     </row>
-    <row r="61" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C61" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B62" s="24" t="s">
         <v>0</v>
       </c>
@@ -13283,7 +13293,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C63" s="8" t="s">
         <v>2</v>
       </c>
@@ -13374,7 +13384,7 @@
       </c>
       <c r="AA63" s="5"/>
     </row>
-    <row r="64" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C64" s="9" t="s">
         <v>38</v>
       </c>
@@ -13470,7 +13480,7 @@
         <v>10.88</v>
       </c>
     </row>
-    <row r="65" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B65" s="15" t="s">
         <v>55</v>
       </c>
@@ -13565,7 +13575,7 @@
         <v>10.88</v>
       </c>
     </row>
-    <row r="67" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B67" s="24" t="s">
         <v>41</v>
       </c>
@@ -13607,7 +13617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B68" s="6"/>
       <c r="C68" s="12" t="s">
         <v>43</v>
@@ -13638,7 +13648,7 @@
       <c r="Y68" s="20"/>
       <c r="AA68" s="23"/>
     </row>
-    <row r="69" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B69" s="6"/>
       <c r="C69" s="12" t="s">
         <v>44</v>
@@ -13669,7 +13679,7 @@
       <c r="Y69" s="20"/>
       <c r="AA69" s="23"/>
     </row>
-    <row r="70" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B70" s="6"/>
       <c r="C70" s="12" t="s">
         <v>45</v>
@@ -13700,7 +13710,7 @@
       <c r="Y70" s="20"/>
       <c r="AA70" s="23"/>
     </row>
-    <row r="71" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C71" s="12" t="s">
         <v>46</v>
       </c>
@@ -13741,7 +13751,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C72" s="12" t="s">
         <v>49</v>
       </c>
@@ -13782,7 +13792,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C73" s="8" t="s">
         <v>37</v>
       </c>
@@ -13876,7 +13886,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C74" s="8" t="s">
         <v>2</v>
       </c>
@@ -13967,7 +13977,7 @@
       </c>
       <c r="AA74" s="5"/>
     </row>
-    <row r="75" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C75" s="9" t="s">
         <v>38</v>
       </c>
@@ -14063,7 +14073,7 @@
         <v>5.7120000000000006</v>
       </c>
     </row>
-    <row r="76" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B76" s="15" t="s">
         <v>56</v>
       </c>
@@ -14158,13 +14168,13 @@
         <v>5.7120000000000006</v>
       </c>
     </row>
-    <row r="79" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C79" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B80" s="24" t="s">
         <v>0</v>
       </c>
@@ -14208,7 +14218,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="81" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C81" s="8" t="s">
         <v>2</v>
       </c>
@@ -14299,7 +14309,7 @@
       </c>
       <c r="AA81" s="5"/>
     </row>
-    <row r="82" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C82" s="9" t="s">
         <v>38</v>
       </c>
@@ -14395,7 +14405,7 @@
         <v>7.7519999999999998</v>
       </c>
     </row>
-    <row r="83" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B83" s="15" t="s">
         <v>60</v>
       </c>
@@ -14490,7 +14500,7 @@
         <v>7.7519999999999998</v>
       </c>
     </row>
-    <row r="85" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B85" s="24" t="s">
         <v>41</v>
       </c>
@@ -14526,7 +14536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B86" s="6"/>
       <c r="C86" s="12" t="s">
         <v>43</v>
@@ -14557,7 +14567,7 @@
       <c r="Y86" s="20"/>
       <c r="AA86" s="23"/>
     </row>
-    <row r="87" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B87" s="6"/>
       <c r="C87" s="12" t="s">
         <v>44</v>
@@ -14598,7 +14608,7 @@
       <c r="Y87" s="20"/>
       <c r="AA87" s="23"/>
     </row>
-    <row r="88" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B88" s="6"/>
       <c r="C88" s="12" t="s">
         <v>45</v>
@@ -14639,7 +14649,7 @@
       <c r="Y88" s="20"/>
       <c r="AA88" s="23"/>
     </row>
-    <row r="89" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C89" s="12" t="s">
         <v>46</v>
       </c>
@@ -14680,7 +14690,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C90" s="12" t="s">
         <v>49</v>
       </c>
@@ -14721,7 +14731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C91" s="8" t="s">
         <v>37</v>
       </c>
@@ -14815,7 +14825,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="92" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C92" s="8" t="s">
         <v>2</v>
       </c>
@@ -14906,7 +14916,7 @@
       </c>
       <c r="AA92" s="5"/>
     </row>
-    <row r="93" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C93" s="9" t="s">
         <v>38</v>
       </c>
@@ -15002,7 +15012,7 @@
         <v>7.4120000000000008</v>
       </c>
     </row>
-    <row r="94" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B94" s="15" t="s">
         <v>61</v>
       </c>
@@ -15097,13 +15107,13 @@
         <v>7.4120000000000008</v>
       </c>
     </row>
-    <row r="97" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C97" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D97" s="3"/>
     </row>
-    <row r="98" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B98" s="24" t="s">
         <v>0</v>
       </c>
@@ -15145,7 +15155,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="99" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C99" s="8" t="s">
         <v>2</v>
       </c>
@@ -15236,7 +15246,7 @@
       </c>
       <c r="AA99" s="5"/>
     </row>
-    <row r="100" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C100" s="9" t="s">
         <v>38</v>
       </c>
@@ -15332,7 +15342,7 @@
         <v>8.0240000000000009</v>
       </c>
     </row>
-    <row r="101" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B101" s="15" t="s">
         <v>63</v>
       </c>
@@ -15427,7 +15437,7 @@
         <v>8.0240000000000009</v>
       </c>
     </row>
-    <row r="103" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B103" s="24" t="s">
         <v>41</v>
       </c>
@@ -15473,7 +15483,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B104" s="6"/>
       <c r="C104" s="12" t="s">
         <v>43</v>
@@ -15514,7 +15524,7 @@
       </c>
       <c r="AA104" s="23"/>
     </row>
-    <row r="105" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B105" s="6"/>
       <c r="C105" s="12" t="s">
         <v>44</v>
@@ -15553,7 +15563,7 @@
       </c>
       <c r="AA105" s="23"/>
     </row>
-    <row r="106" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B106" s="6"/>
       <c r="C106" s="12" t="s">
         <v>45</v>
@@ -15590,7 +15600,7 @@
       </c>
       <c r="AA106" s="23"/>
     </row>
-    <row r="107" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C107" s="12" t="s">
         <v>46</v>
       </c>
@@ -15627,7 +15637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C108" s="12" t="s">
         <v>49</v>
       </c>
@@ -15668,7 +15678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C109" s="8" t="s">
         <v>37</v>
       </c>
@@ -15762,7 +15772,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C110" s="8" t="s">
         <v>2</v>
       </c>
@@ -15853,7 +15863,7 @@
       </c>
       <c r="AA110" s="5"/>
     </row>
-    <row r="111" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C111" s="9" t="s">
         <v>38</v>
       </c>
@@ -15949,7 +15959,7 @@
         <v>7.1400000000000006</v>
       </c>
     </row>
-    <row r="112" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B112" s="15" t="s">
         <v>64</v>
       </c>
@@ -16061,7 +16071,7 @@
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16076,7 +16086,7 @@
       <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16091,7 +16101,7 @@
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16106,7 +16116,7 @@
       <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>